<commit_message>
added some more classes
</commit_message>
<xml_diff>
--- a/target/read2.xlsx
+++ b/target/read2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Praveen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Praveen\eclipse-workspace\SRYA\EXEMAVEN\target\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,12 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>praveen</t>
-  </si>
-  <si>
-    <t>chennai</t>
-  </si>
-  <si>
     <t>ram</t>
   </si>
   <si>
@@ -48,6 +42,12 @@
   </si>
   <si>
     <t>salem</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
   </si>
 </sst>
 </file>
@@ -369,54 +369,46 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>34693</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>34855</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>34825</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>34959</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>